<commit_message>
Fix template tests - fix input data and ref value
Signed-off-by: David Kroon <david.kroon@ortec-finance.com>
</commit_message>
<xml_diff>
--- a/examples/data/20220306 ITR Tool Sample Data.xlsx
+++ b/examples/data/20220306 ITR Tool Sample Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR/examples/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ITR\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA993AED-72FB-5B43-BBFE-2C13DC33FA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BBB92D-D9B9-46FE-9CB4-7E2469FB2E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="15560" windowWidth="44560" windowHeight="22440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="5" r:id="rId1"/>
@@ -1650,7 +1650,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -2156,7 +2156,7 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -3368,7 +3368,7 @@
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="20" spans="12:18">
       <c r="L20" s="2"/>
@@ -3396,34 +3396,34 @@
   </sheetPr>
   <dimension ref="A1:AZ53"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A44" sqref="A44:C44"/>
+      <selection pane="bottomRight" activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="24"/>
-    <col min="7" max="7" width="16.5" style="4"/>
-    <col min="9" max="9" width="16.5" style="5"/>
-    <col min="14" max="14" width="25.83203125" customWidth="1"/>
-    <col min="15" max="15" width="25.83203125" style="60" customWidth="1"/>
-    <col min="16" max="16" width="22.1640625" customWidth="1"/>
-    <col min="17" max="21" width="16.5" customWidth="1"/>
-    <col min="22" max="22" width="16.5" style="2" customWidth="1"/>
-    <col min="23" max="23" width="16.5" style="36" customWidth="1"/>
-    <col min="24" max="29" width="16.5" style="2" customWidth="1"/>
-    <col min="30" max="30" width="16.5" style="36" customWidth="1"/>
-    <col min="31" max="37" width="16.5" style="2" customWidth="1"/>
-    <col min="38" max="44" width="16.5" style="2"/>
-    <col min="45" max="49" width="16.83203125" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="16.5" style="2"/>
+    <col min="2" max="2" width="25.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="24"/>
+    <col min="7" max="7" width="16.44140625" style="4"/>
+    <col min="9" max="9" width="16.44140625" style="5"/>
+    <col min="14" max="14" width="25.77734375" customWidth="1"/>
+    <col min="15" max="15" width="25.77734375" style="60" customWidth="1"/>
+    <col min="16" max="16" width="22.109375" customWidth="1"/>
+    <col min="17" max="21" width="16.44140625" customWidth="1"/>
+    <col min="22" max="22" width="16.44140625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="16.44140625" style="36" customWidth="1"/>
+    <col min="24" max="29" width="16.44140625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="16.44140625" style="36" customWidth="1"/>
+    <col min="31" max="37" width="16.44140625" style="2" customWidth="1"/>
+    <col min="38" max="44" width="16.44140625" style="2"/>
+    <col min="45" max="49" width="16.77734375" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="16.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" ht="16">
+    <row r="1" spans="1:52" s="3" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>83985.94</v>
       </c>
       <c r="AV2" s="60">
-        <v>759043.55</v>
+        <v>75904.354999999996</v>
       </c>
       <c r="AW2" s="60">
         <v>75271.521999999997</v>
@@ -8464,19 +8464,19 @@
       <selection pane="bottomRight" activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="29.33203125" style="60" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="60"/>
-    <col min="4" max="4" width="16.5" style="26"/>
-    <col min="5" max="5" width="17.5" style="26" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="60"/>
+    <col min="4" max="4" width="16.44140625" style="26"/>
+    <col min="5" max="5" width="17.44140625" style="26" customWidth="1"/>
     <col min="6" max="7" width="24" style="60" customWidth="1"/>
-    <col min="8" max="8" width="22.5" style="20" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" style="20" customWidth="1"/>
     <col min="9" max="9" width="23.33203125" style="60" customWidth="1"/>
     <col min="10" max="10" width="24" style="60" customWidth="1"/>
     <col min="11" max="11" width="19.33203125" style="60" customWidth="1"/>
-    <col min="12" max="12" width="21.5" style="60" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -10577,17 +10577,17 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" style="34" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="21.6640625" style="51" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" customWidth="1"/>
     <col min="8" max="8" width="87.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
       <c r="A1" s="38" t="s">
         <v>12</v>
       </c>
@@ -10607,7 +10607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16">
+    <row r="2" spans="1:6">
       <c r="A2" s="40" t="s">
         <v>13</v>
       </c>
@@ -10627,7 +10627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16">
+    <row r="3" spans="1:6">
       <c r="A3" s="40" t="s">
         <v>13</v>
       </c>
@@ -10647,7 +10647,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="32">
+    <row r="4" spans="1:6" ht="43.2">
       <c r="A4" s="40" t="s">
         <v>13</v>
       </c>
@@ -10667,7 +10667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="32">
+    <row r="5" spans="1:6" ht="28.8">
       <c r="A5" s="40" t="s">
         <v>13</v>
       </c>
@@ -10687,7 +10687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="48">
+    <row r="6" spans="1:6" ht="43.2">
       <c r="A6" s="40" t="s">
         <v>13</v>
       </c>
@@ -10707,7 +10707,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16">
+    <row r="7" spans="1:6">
       <c r="A7" s="40" t="s">
         <v>13</v>
       </c>
@@ -10727,7 +10727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16">
+    <row r="8" spans="1:6">
       <c r="A8" s="40" t="s">
         <v>13</v>
       </c>
@@ -10747,7 +10747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="32">
+    <row r="9" spans="1:6" ht="28.8">
       <c r="A9" s="40" t="s">
         <v>13</v>
       </c>
@@ -10767,7 +10767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6">
       <c r="A10" s="40" t="s">
         <v>13</v>
       </c>
@@ -10787,7 +10787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16">
+    <row r="11" spans="1:6">
       <c r="A11" s="40" t="s">
         <v>13</v>
       </c>
@@ -10807,7 +10807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16">
+    <row r="12" spans="1:6">
       <c r="A12" s="40" t="s">
         <v>13</v>
       </c>
@@ -10827,7 +10827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16">
+    <row r="13" spans="1:6">
       <c r="A13" s="40" t="s">
         <v>13</v>
       </c>
@@ -10847,7 +10847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="32">
+    <row r="14" spans="1:6" ht="28.8">
       <c r="A14" s="40" t="s">
         <v>13</v>
       </c>
@@ -10867,7 +10867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16">
+    <row r="15" spans="1:6">
       <c r="A15" s="40" t="s">
         <v>13</v>
       </c>
@@ -10927,7 +10927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="32">
+    <row r="18" spans="1:6" ht="28.8">
       <c r="A18" s="31" t="s">
         <v>15</v>
       </c>
@@ -10947,7 +10947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="32">
+    <row r="19" spans="1:6" ht="28.8">
       <c r="A19" s="31" t="s">
         <v>15</v>
       </c>
@@ -10967,7 +10967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="32">
+    <row r="20" spans="1:6" ht="28.8">
       <c r="A20" s="31" t="s">
         <v>15</v>
       </c>
@@ -10987,7 +10987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="32">
+    <row r="21" spans="1:6" ht="28.8">
       <c r="A21" s="31" t="s">
         <v>15</v>
       </c>
@@ -11007,7 +11007,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="32">
+    <row r="22" spans="1:6" ht="28.8">
       <c r="A22" s="31" t="s">
         <v>15</v>
       </c>
@@ -11027,7 +11027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="32">
+    <row r="23" spans="1:6" ht="28.8">
       <c r="A23" s="31" t="s">
         <v>15</v>
       </c>
@@ -11047,7 +11047,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="48">
+    <row r="24" spans="1:6" ht="43.2">
       <c r="A24" s="31" t="s">
         <v>15</v>
       </c>
@@ -11067,7 +11067,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="32">
+    <row r="25" spans="1:6" ht="28.8">
       <c r="A25" s="31" t="s">
         <v>15</v>
       </c>
@@ -11087,7 +11087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="32">
+    <row r="26" spans="1:6" ht="28.8">
       <c r="A26" s="31" t="s">
         <v>15</v>
       </c>
@@ -11107,7 +11107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="32">
+    <row r="27" spans="1:6" ht="28.8">
       <c r="A27" s="31" t="s">
         <v>15</v>
       </c>
@@ -11127,7 +11127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="32">
+    <row r="28" spans="1:6" ht="28.8">
       <c r="A28" s="31" t="s">
         <v>15</v>
       </c>
@@ -11147,7 +11147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="32">
+    <row r="29" spans="1:6" ht="28.8">
       <c r="A29" s="31" t="s">
         <v>15</v>
       </c>
@@ -11167,7 +11167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="32">
+    <row r="30" spans="1:6" ht="28.8">
       <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
@@ -11187,7 +11187,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="48">
+    <row r="31" spans="1:6" ht="43.2">
       <c r="A31" s="31" t="s">
         <v>15</v>
       </c>
@@ -11207,7 +11207,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="32">
+    <row r="32" spans="1:6" ht="28.8">
       <c r="A32" s="31" t="s">
         <v>15</v>
       </c>
@@ -11227,7 +11227,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="32">
+    <row r="33" spans="1:6" ht="28.8">
       <c r="A33" s="31" t="s">
         <v>15</v>
       </c>
@@ -11247,7 +11247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="32">
+    <row r="34" spans="1:6" ht="28.8">
       <c r="A34" s="31" t="s">
         <v>15</v>
       </c>
@@ -11267,7 +11267,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="32">
+    <row r="35" spans="1:6" ht="28.8">
       <c r="A35" s="31" t="s">
         <v>15</v>
       </c>
@@ -11287,7 +11287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="32">
+    <row r="36" spans="1:6" ht="28.8">
       <c r="A36" s="31" t="s">
         <v>15</v>
       </c>
@@ -11307,7 +11307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="32">
+    <row r="37" spans="1:6" ht="28.8">
       <c r="A37" s="31" t="s">
         <v>15</v>
       </c>
@@ -11327,7 +11327,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="48">
+    <row r="38" spans="1:6" ht="43.2">
       <c r="A38" s="31" t="s">
         <v>15</v>
       </c>
@@ -11347,7 +11347,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="32">
+    <row r="39" spans="1:6" ht="28.8">
       <c r="A39" s="31" t="s">
         <v>15</v>
       </c>
@@ -11367,7 +11367,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="32">
+    <row r="40" spans="1:6" ht="28.8">
       <c r="A40" s="31" t="s">
         <v>15</v>
       </c>
@@ -11387,7 +11387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="32">
+    <row r="41" spans="1:6" ht="28.8">
       <c r="A41" s="31" t="s">
         <v>15</v>
       </c>
@@ -11407,7 +11407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="32">
+    <row r="42" spans="1:6" ht="28.8">
       <c r="A42" s="31" t="s">
         <v>15</v>
       </c>
@@ -11427,7 +11427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="32">
+    <row r="43" spans="1:6" ht="28.8">
       <c r="A43" s="31" t="s">
         <v>15</v>
       </c>
@@ -11447,7 +11447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="32">
+    <row r="44" spans="1:6" ht="28.8">
       <c r="A44" s="31" t="s">
         <v>15</v>
       </c>
@@ -11467,7 +11467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="48">
+    <row r="45" spans="1:6" ht="43.2">
       <c r="A45" s="31" t="s">
         <v>15</v>
       </c>
@@ -11487,7 +11487,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="32">
+    <row r="46" spans="1:6" ht="28.8">
       <c r="A46" s="50" t="s">
         <v>74</v>
       </c>
@@ -11507,7 +11507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="32">
+    <row r="47" spans="1:6" ht="28.8">
       <c r="A47" s="50" t="s">
         <v>74</v>
       </c>
@@ -11527,7 +11527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="32">
+    <row r="48" spans="1:6" ht="28.8">
       <c r="A48" s="50" t="s">
         <v>74</v>
       </c>
@@ -11547,7 +11547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="32">
+    <row r="49" spans="1:6" ht="28.8">
       <c r="A49" s="50" t="s">
         <v>74</v>
       </c>
@@ -11567,7 +11567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="32">
+    <row r="50" spans="1:6" ht="28.8">
       <c r="A50" s="50" t="s">
         <v>74</v>
       </c>
@@ -11587,7 +11587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="32">
+    <row r="51" spans="1:6" ht="28.8">
       <c r="A51" s="44" t="s">
         <v>14</v>
       </c>
@@ -11607,7 +11607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="48">
+    <row r="52" spans="1:6" ht="43.2">
       <c r="A52" s="44" t="s">
         <v>14</v>
       </c>
@@ -11627,7 +11627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="16">
+    <row r="53" spans="1:6">
       <c r="A53" s="44" t="s">
         <v>14</v>
       </c>
@@ -11647,7 +11647,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="16">
+    <row r="54" spans="1:6">
       <c r="A54" s="44" t="s">
         <v>14</v>
       </c>
@@ -11667,7 +11667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="80">
+    <row r="55" spans="1:6" ht="72">
       <c r="A55" s="44" t="s">
         <v>14</v>
       </c>
@@ -11687,7 +11687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="64">
+    <row r="56" spans="1:6" ht="72">
       <c r="A56" s="44" t="s">
         <v>14</v>
       </c>
@@ -11707,7 +11707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="16">
+    <row r="57" spans="1:6">
       <c r="A57" s="44" t="s">
         <v>14</v>
       </c>
@@ -11727,7 +11727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="32">
+    <row r="58" spans="1:6" ht="28.8">
       <c r="A58" s="44" t="s">
         <v>14</v>
       </c>
@@ -11747,7 +11747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="48">
+    <row r="59" spans="1:6" ht="43.2">
       <c r="A59" s="45" t="s">
         <v>102</v>
       </c>
@@ -11781,16 +11781,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F8BFE4-8461-B541-8467-258963D3527B}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" customWidth="1"/>
+    <col min="1" max="1" width="40.77734375" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="60" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -11825,7 +11825,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(35000,250000)</f>
-        <v>156184</v>
+        <v>240110</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11843,7 +11843,7 @@
       </c>
       <c r="E3" s="60">
         <f t="shared" ref="E3:E45" ca="1" si="0">RANDBETWEEN(35000,250000)</f>
-        <v>121116</v>
+        <v>181765</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -11861,7 +11861,7 @@
       </c>
       <c r="E4" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>47316</v>
+        <v>61005</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -11879,7 +11879,7 @@
       </c>
       <c r="E5" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>223215</v>
+        <v>154501</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -11897,7 +11897,7 @@
       </c>
       <c r="E6" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>224514</v>
+        <v>149431</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -11915,7 +11915,7 @@
       </c>
       <c r="E7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>130276</v>
+        <v>139040</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -11933,7 +11933,7 @@
       </c>
       <c r="E8" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>183863</v>
+        <v>101009</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -11951,7 +11951,7 @@
       </c>
       <c r="E9" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>149008</v>
+        <v>178835</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -11969,7 +11969,7 @@
       </c>
       <c r="E10" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>119429</v>
+        <v>66099</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -11987,7 +11987,7 @@
       </c>
       <c r="E11" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>175333</v>
+        <v>74872</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -12005,7 +12005,7 @@
       </c>
       <c r="E12" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>202612</v>
+        <v>138045</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -12023,7 +12023,7 @@
       </c>
       <c r="E13" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>49914</v>
+        <v>165726</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -12041,7 +12041,7 @@
       </c>
       <c r="E14" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>233108</v>
+        <v>129283</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -12059,7 +12059,7 @@
       </c>
       <c r="E15" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>84518</v>
+        <v>47941</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -12077,7 +12077,7 @@
       </c>
       <c r="E16" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>56784</v>
+        <v>183791</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -12095,7 +12095,7 @@
       </c>
       <c r="E17" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>118715</v>
+        <v>178679</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -12113,7 +12113,7 @@
       </c>
       <c r="E18" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>55497</v>
+        <v>211530</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -12131,7 +12131,7 @@
       </c>
       <c r="E19" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>248863</v>
+        <v>86018</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -12149,7 +12149,7 @@
       </c>
       <c r="E20" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>228198</v>
+        <v>145715</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -12167,7 +12167,7 @@
       </c>
       <c r="E21" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>59341</v>
+        <v>82925</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -12185,7 +12185,7 @@
       </c>
       <c r="E22" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>177653</v>
+        <v>176740</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -12203,7 +12203,7 @@
       </c>
       <c r="E23" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>96576</v>
+        <v>131498</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -12221,7 +12221,7 @@
       </c>
       <c r="E24" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>177368</v>
+        <v>102589</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -12239,7 +12239,7 @@
       </c>
       <c r="E25" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>168914</v>
+        <v>247573</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -12257,7 +12257,7 @@
       </c>
       <c r="E26" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>93969</v>
+        <v>129523</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -12275,7 +12275,7 @@
       </c>
       <c r="E27" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>177231</v>
+        <v>79959</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -12293,7 +12293,7 @@
       </c>
       <c r="E28" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>159501</v>
+        <v>56770</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -12311,7 +12311,7 @@
       </c>
       <c r="E29" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>112012</v>
+        <v>124278</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -12329,7 +12329,7 @@
       </c>
       <c r="E30" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>142745</v>
+        <v>64330</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -12347,7 +12347,7 @@
       </c>
       <c r="E31" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>84151</v>
+        <v>194452</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -12365,7 +12365,7 @@
       </c>
       <c r="E32" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>69662</v>
+        <v>36825</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -12383,7 +12383,7 @@
       </c>
       <c r="E33" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>138126</v>
+        <v>84112</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -12401,7 +12401,7 @@
       </c>
       <c r="E34" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>226744</v>
+        <v>50359</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -12419,7 +12419,7 @@
       </c>
       <c r="E35" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>148669</v>
+        <v>135998</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -12437,7 +12437,7 @@
       </c>
       <c r="E36" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>131916</v>
+        <v>153563</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -12455,7 +12455,7 @@
       </c>
       <c r="E37" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>247557</v>
+        <v>102150</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -12473,7 +12473,7 @@
       </c>
       <c r="E38" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>245583</v>
+        <v>165034</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -12491,7 +12491,7 @@
       </c>
       <c r="E39" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>177079</v>
+        <v>219239</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -12509,7 +12509,7 @@
       </c>
       <c r="E40" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>141686</v>
+        <v>136196</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -12527,7 +12527,7 @@
       </c>
       <c r="E41" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>143651</v>
+        <v>156989</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -12545,7 +12545,7 @@
       </c>
       <c r="E42" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>89816</v>
+        <v>245940</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -12563,7 +12563,7 @@
       </c>
       <c r="E43" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>141313</v>
+        <v>176410</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="60" customFormat="1">
@@ -12581,7 +12581,7 @@
       </c>
       <c r="E44" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>87867</v>
+        <v>212025</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -12599,7 +12599,7 @@
       </c>
       <c r="E45" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>217156</v>
+        <v>108624</v>
       </c>
     </row>
   </sheetData>
@@ -12617,6 +12617,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB6CE2092F7CDA4FBA49881696A89DE0" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b5918a5add965903052caa4f280154e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="020ef37c-4094-40f4-bf82-41b1d62e0e53" xmlns:ns4="40408af7-2a3f-48ae-b560-b937464d5fc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55d586a85da155bcad137d4f3c4349ba" ns3:_="" ns4:_="">
     <xsd:import namespace="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
@@ -12833,12 +12839,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EA39C3-A15D-48B6-A2C6-B0C6753DDE50}">
   <ds:schemaRefs>
@@ -12848,6 +12848,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C61229-62A1-4F5F-B8F8-172CE6F3C2F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12864,21 +12881,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9247F93A-D89B-4D3E-A390-CCD57A0A6ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="40408af7-2a3f-48ae-b560-b937464d5fc3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="020ef37c-4094-40f4-bf82-41b1d62e0e53"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>